<commit_message>
Lade till en liten hög med saker
Collider, level
Ändrade lite ko i olika filer
</commit_message>
<xml_diff>
--- a/Project Plan.xlsx
+++ b/Project Plan.xlsx
@@ -453,7 +453,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -611,7 +611,7 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C14" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
.mp3->.wav, fixat med MenuState
(fortsätter efter sömn)
</commit_message>
<xml_diff>
--- a/Project Plan.xlsx
+++ b/Project Plan.xlsx
@@ -453,7 +453,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -479,7 +479,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
         <v>19</v>
@@ -490,7 +490,7 @@
         <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
         <v>20</v>
@@ -501,7 +501,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
         <v>19</v>
@@ -512,7 +512,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
         <v>19</v>
@@ -523,7 +523,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
         <v>20</v>
@@ -534,7 +534,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
         <v>19</v>
@@ -545,7 +545,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
         <v>20</v>
@@ -556,7 +556,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
         <v>20</v>

</xml_diff>